<commit_message>
v1.1 Added Navigation feature to the RTM
</commit_message>
<xml_diff>
--- a/LH_RTM/LH_RTM.xlsx
+++ b/LH_RTM/LH_RTM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce4e295319cf0be1/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607238D3-5B03-4110-BFD8-671560B87574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7262910-F7CA-4F5D-A902-C01217696186}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRS_to_SRS" sheetId="4" r:id="rId1"/>
@@ -20,22 +20,11 @@
     <sheet name="README" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
   <si>
     <t>SRS ID</t>
   </si>
@@ -230,12 +219,87 @@
   <si>
     <t>15/4/2025</t>
   </si>
+  <si>
+    <t>LH-CRS-NAVIGATION-001</t>
+  </si>
+  <si>
+    <t>users should be able to navigate between different content categories</t>
+  </si>
+  <si>
+    <t>SRS-NAV-001</t>
+  </si>
+  <si>
+    <t>The system allow users to navigate between four predefined content categories  ( ‘Sports’, ‘Scientific’,'Health','Economy').</t>
+  </si>
+  <si>
+    <t>LH-CRS-NAVIGATION-002</t>
+  </si>
+  <si>
+    <t>The website must include a header navigation bar with tabs for each section and dropdowns for subsections.</t>
+  </si>
+  <si>
+    <t>SRS-NAV-002</t>
+  </si>
+  <si>
+    <t>The system include a header navigation bar with tabs for each section and clickable dropdowns for subsections.</t>
+  </si>
+  <si>
+    <t>LH-CRS-NAVIGATION-003</t>
+  </si>
+  <si>
+    <t>The website must include exactly 4 content categories.</t>
+  </si>
+  <si>
+    <t>SRS-NAV-003</t>
+  </si>
+  <si>
+    <t>The system shall restrict content categories to exactly four (4) with no additions/deletions by users.</t>
+  </si>
+  <si>
+    <t>NAVIGATION</t>
+  </si>
+  <si>
+    <t>LH-TC-NAVIGATION-001</t>
+  </si>
+  <si>
+    <t>Verify that the user can navigate between all four predefined content categories from the main interface.</t>
+  </si>
+  <si>
+    <t>LH-TC-NAVIGATION-002</t>
+  </si>
+  <si>
+    <t>Validate that the header navigation bar displays tabs for each category and provides dropdowns for subsections.</t>
+  </si>
+  <si>
+    <t>LH-TC-NAVIGATION-003</t>
+  </si>
+  <si>
+    <t>Verify that categories without any subsections do not show a dropdown and still function correctly when clicked.</t>
+  </si>
+  <si>
+    <t>LH-TC-NAVIGATION-004</t>
+  </si>
+  <si>
+    <t>Verify that users cannot add or remove categories through any available means and that the system does not expose any interfaces to modify the four predefined categories.</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>Gehad Ashry</t>
+  </si>
+  <si>
+    <t>Added Navigation Feature after reviewer verification</t>
+  </si>
+  <si>
+    <t>21/4/2025</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,8 +401,38 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,8 +487,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -493,11 +593,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -517,75 +641,122 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="13" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="13" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="13" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="13" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -603,6 +774,61 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1145,39 +1371,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA209DF0-93B8-4D30-B2FB-414CDB7D7F90}" name="Table27" displayName="Table27" ref="A1:F12" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
-  <autoFilter ref="A1:F12" xr:uid="{4F1FF083-FA79-4CE2-8554-13F8E83AEA9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA209DF0-93B8-4D30-B2FB-414CDB7D7F90}" name="Table27" displayName="Table27" ref="A1:F17" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26">
+  <autoFilter ref="A1:F17" xr:uid="{4F1FF083-FA79-4CE2-8554-13F8E83AEA9B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6CA57970-FD83-47B6-B26A-137D9968C172}" name="CRS ID " dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{C2FBD084-DDFD-46ED-98E5-7767B2EE7532}" name="CRS Description" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{5F296C86-F482-475B-9DDA-2396D2A96582}" name="SRS ID" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{DC89E710-B8E5-4EE0-ACAF-AD1B3CC3BD8A}" name="SRS Description" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{1FBD9013-D7E8-4B61-AFDA-B41F2878B297}" name="Status (CRS-SRS)" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{0EF77139-5449-4C44-894F-C1EDEBFD8E5E}" name="Comments/Gaps" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{6CA57970-FD83-47B6-B26A-137D9968C172}" name="CRS ID " dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{C2FBD084-DDFD-46ED-98E5-7767B2EE7532}" name="CRS Description" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{5F296C86-F482-475B-9DDA-2396D2A96582}" name="SRS ID" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{DC89E710-B8E5-4EE0-ACAF-AD1B3CC3BD8A}" name="SRS Description" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{1FBD9013-D7E8-4B61-AFDA-B41F2878B297}" name="Status (CRS-SRS)" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{0EF77139-5449-4C44-894F-C1EDEBFD8E5E}" name="Comments/Gaps" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AF4E328A-81DE-4BBA-BCF0-691C6E1489E8}" name="Table26" displayName="Table26" ref="A1:F15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
-  <autoFilter ref="A1:F15" xr:uid="{4F1FF083-FA79-4CE2-8554-13F8E83AEA9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AF4E328A-81DE-4BBA-BCF0-691C6E1489E8}" name="Table26" displayName="Table26" ref="A1:F22" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+  <autoFilter ref="A1:F22" xr:uid="{4F1FF083-FA79-4CE2-8554-13F8E83AEA9B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A54AB838-1B45-4783-A1A8-2EC0D7994179}" name="SRS ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F4498237-0ED4-49E6-A0D6-70E81329E6FB}" name="SRS Description" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{0EC4E366-CD72-4E09-ABF8-DBB51D5C7CBE}" name="Test Case ID" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{86647B66-A330-4B5B-A580-5CE73E1A93D4}" name="Test Description" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{C1F47C5E-CDEF-41A5-838F-10820A19570C}" name="Test Result" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{0E603383-6D99-4B7E-8571-905C4776D635}" name="Status (Test)" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{A54AB838-1B45-4783-A1A8-2EC0D7994179}" name="SRS ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{F4498237-0ED4-49E6-A0D6-70E81329E6FB}" name="SRS Description" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{0EC4E366-CD72-4E09-ABF8-DBB51D5C7CBE}" name="Test Case ID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{86647B66-A330-4B5B-A580-5CE73E1A93D4}" name="Test Description" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{C1F47C5E-CDEF-41A5-838F-10820A19570C}" name="Test Result" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{0E603383-6D99-4B7E-8571-905C4776D635}" name="Status (Test)" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1215,9 +1441,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1250,9 +1476,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1285,9 +1528,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1461,25 +1721,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F785F3-5151-4BC1-9CA2-DE1F9E7BDBB0}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="2"/>
-    <col min="2" max="2" width="40.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="2"/>
+    <col min="1" max="1" width="25.7109375" style="2"/>
+    <col min="2" max="2" width="40.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="2"/>
     <col min="4" max="4" width="46" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="25.6640625" style="2"/>
+    <col min="5" max="5" width="17.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="25.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="40.5">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -1499,7 +1759,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="25.5">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1515,11 +1775,11 @@
       <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="38.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1535,9 +1795,9 @@
       <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="38.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1553,38 +1813,177 @@
       <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:11" ht="25.5">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" customFormat="1" ht="15">
+      <c r="A6" s="31"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="1:11" customFormat="1" ht="38.25">
+      <c r="A7" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+    </row>
+    <row r="8" spans="1:11" customFormat="1" ht="38.25">
+      <c r="A8" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="33"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+    </row>
+    <row r="9" spans="1:11" customFormat="1" ht="38.25">
+      <c r="A9" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="37"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+    </row>
+    <row r="10" spans="1:11" customFormat="1" ht="15">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G7:G9"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" priority="2">
+  <conditionalFormatting sqref="A11:G15 A1:F4 A11:F1048576 B7:E8">
+    <cfRule type="expression" priority="11">
       <formula>ISBLANK($C2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:XFD2 A6:XFD1048576 A3:F5 H3:XFD5">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="A2:XFD2 A3:F5 H3:XFD5 A11:XFD1048576">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>ISBLANK($C2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:F5">
+    <cfRule type="expression" priority="14">
+      <formula>ISBLANK($C11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>ISBLANK($C7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:E9">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>ISBLANK($C7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:C9">
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>ISBLANK($C7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:B9">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>ISBLANK($C7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:D9">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>ISBLANK($C7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:E9">
+    <cfRule type="expression" priority="17">
+      <formula>ISBLANK($C11)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1593,31 +1992,32 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29502484-95DD-49B9-AE58-DBAB74E3B005}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="2"/>
-    <col min="2" max="2" width="50.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.33203125" style="2" customWidth="1"/>
-    <col min="4" max="6" width="25.6640625" style="2"/>
-    <col min="7" max="7" width="23.109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="25.6640625" style="2"/>
+    <col min="1" max="1" width="25.7109375" style="2"/>
+    <col min="2" max="2" width="50.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" style="2" customWidth="1"/>
+    <col min="4" max="6" width="25.7109375" style="2"/>
+    <col min="7" max="7" width="23.140625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="25.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +2037,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="38.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1650,11 +2050,11 @@
       <c r="D2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="25.5">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1667,9 +2067,9 @@
       <c r="D3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" ht="25.5">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1682,9 +2082,9 @@
       <c r="D4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:7" ht="25.5">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1697,9 +2097,9 @@
       <c r="D5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" ht="38.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1712,9 +2112,9 @@
       <c r="D6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" ht="38.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1727,9 +2127,9 @@
       <c r="D7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" ht="25.5">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1742,9 +2142,9 @@
       <c r="D8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1757,9 +2157,9 @@
       <c r="D9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" ht="38.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1772,9 +2172,9 @@
       <c r="D10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" ht="38.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1787,9 +2187,9 @@
       <c r="D11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" ht="25.5">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1802,9 +2202,9 @@
       <c r="D12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" ht="25.5">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1817,9 +2217,9 @@
       <c r="D13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" ht="38.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1832,9 +2232,9 @@
       <c r="D14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" ht="25.5">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1849,18 +2249,115 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="10"/>
+      <c r="G15" s="27"/>
+    </row>
+    <row r="16" spans="1:7" customFormat="1" ht="15">
+      <c r="A16" s="42"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="31"/>
+    </row>
+    <row r="17" spans="1:7" customFormat="1" ht="51">
+      <c r="A17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" customFormat="1" ht="63.75">
+      <c r="A18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="47"/>
+    </row>
+    <row r="19" spans="1:7" customFormat="1" ht="51">
+      <c r="A19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="47"/>
+    </row>
+    <row r="20" spans="1:7" customFormat="1" ht="76.5">
+      <c r="A20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="47"/>
+    </row>
+    <row r="21" spans="1:7" customFormat="1" ht="15">
+      <c r="A21" s="42"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="31"/>
+    </row>
+    <row r="22" spans="1:7" customFormat="1" ht="15">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="G2:G15"/>
+    <mergeCell ref="G17:G20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1887,80 +2384,80 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="21.88671875" style="14"/>
+    <col min="1" max="16384" width="21.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:2" ht="21">
+      <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="14">
-        <f>COUNTA(CRS_to_SRS!A2:A100)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="B2" s="8">
+        <f>COUNTA(CRS_to_SRS!A2:A105)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="14">
-        <f>COUNTA(SRS_to_Test!A2:A100)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="B3" s="8">
+        <f>COUNTA(SRS_to_Test!A2:A107)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="14">
-        <f>COUNTIF(SRS_to_Test!E2:E100, "Pass")</f>
+      <c r="B4" s="8">
+        <f>COUNTIF(SRS_to_Test!E2:E107, "Pass")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="8">
         <f>(B4/B3)*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+    <row r="6" spans="1:2" s="9" customFormat="1"/>
+    <row r="7" spans="1:2" ht="21">
+      <c r="A7" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="14">
-        <f>COUNTIF(CRS_to_SRS!C2:C100, "")</f>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="B8" s="8">
+        <f>COUNTIF(CRS_to_SRS!C2:C105, "")</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="14">
-        <f>COUNTIF(SRS_to_Test!C2:C100, "")</f>
-        <v>85</v>
+      <c r="B9" s="8">
+        <f>COUNTIF(SRS_to_Test!C2:C107, "")</f>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1973,75 +2470,83 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="33.21875" customWidth="1"/>
-    <col min="3" max="3" width="42.77734375" customWidth="1"/>
-    <col min="4" max="4" width="37.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="11" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" ht="20.25">
+      <c r="A1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:6" ht="18.75">
+      <c r="A2" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20" t="s">
+    <row r="3" spans="1:6" ht="37.5">
+      <c r="A3" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="23"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="23"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F10" s="27"/>
-    </row>
-    <row r="17" spans="2:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="F10" s="21"/>
+    </row>
+    <row r="17" spans="2:4" ht="21">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2057,12 +2562,12 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.45" customHeight="1">
       <c r="A1" s="28" t="s">
         <v>43</v>
       </c>
@@ -2070,37 +2575,37 @@
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="28"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="28"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="28"/>
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="28"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="28"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>

</xml_diff>

<commit_message>
v1.4 created Notifications and ID CONSTRAINTS RTM
LH_RTM_UPDATE_050
created Notifications and ID CONSTRAINTS RTM (CRS to SRS) and (SRS to Test Cases)
</commit_message>
<xml_diff>
--- a/LH_RTM/LH_RTM.xlsx
+++ b/LH_RTM/LH_RTM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8935768D-800B-425E-96D0-C19EBC3D7F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRS_to_SRS" sheetId="4" r:id="rId1"/>
@@ -18,12 +19,25 @@
     <sheet name="Version_History" sheetId="5" r:id="rId4"/>
     <sheet name="README" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="223">
   <si>
     <t>SRS ID</t>
   </si>
@@ -569,9 +583,6 @@
     <t>TC-PUB-018</t>
   </si>
   <si>
-    <t>TC-PUB-019</t>
-  </si>
-  <si>
     <t>Verify UI Buttons for Publishing Options</t>
   </si>
   <si>
@@ -626,9 +637,6 @@
     <t>Validate Valid Audio Format (.mp3 Only)</t>
   </si>
   <si>
-    <t>Validate Invalid Audio Format (e.g., .wav)</t>
-  </si>
-  <si>
     <t>RS-PUB-001.1</t>
   </si>
   <si>
@@ -645,13 +653,122 @@
   </si>
   <si>
     <t>created PUBLISH&amp;UPLOAD RTM (CRS to SRS) and (SRS to Test Cases)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS-ID-001
+</t>
+  </si>
+  <si>
+    <t>LH-TC-IDCONSTRAINTS_001</t>
+  </si>
+  <si>
+    <t>Verifying that each user receives a unique ID upon registration</t>
+  </si>
+  <si>
+    <t>SRS-ID-002.1</t>
+  </si>
+  <si>
+    <t>SRS-ID-002.3</t>
+  </si>
+  <si>
+    <t>LH-TC-IDCONSTRAINTS_002</t>
+  </si>
+  <si>
+    <t>LH-TC-IDCONSTRAINTS_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensuring generated user IDs follow the required format UXXX.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Checking that user IDs are generated sequentially.</t>
+  </si>
+  <si>
+    <t>User IDs shall be generated upon registration.</t>
+  </si>
+  <si>
+    <t>The system shall automatically generate a unique user ID for each new registration in the format UXXX (ex:U001)</t>
+  </si>
+  <si>
+    <t>Generated user IDs shall be stored persistently in the database alongside user details (email, username, etc.)</t>
+  </si>
+  <si>
+    <t>The system shall retrieve the last assigned ID from the database to compute the next sequential ID</t>
+  </si>
+  <si>
+    <t>The system shall allow users to toggle "Follow" on categories, store preferences in the database.</t>
+  </si>
+  <si>
+    <t>The system shall display unread notifications in a bell icon dropdown.</t>
+  </si>
+  <si>
+    <t>LH-TC-NOTIFICATION-001</t>
+  </si>
+  <si>
+    <t>LH-TC-NOTIFICATION-002</t>
+  </si>
+  <si>
+    <t>Testing the functionality of toggling the"Follow" option for categories</t>
+  </si>
+  <si>
+    <t>Testing the ability to display unread notifications via the bell icon dropdown</t>
+  </si>
+  <si>
+    <t>SRS-NOT-001</t>
+  </si>
+  <si>
+    <t>SRS-NOT-002</t>
+  </si>
+  <si>
+    <t>ID CONSTRAINTS</t>
+  </si>
+  <si>
+    <t>LH-CRS-ID-CONSTRAINS-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-ID-CONSTRAINTS-002</t>
+  </si>
+  <si>
+    <t>each user must be assigned a unique user ID after creating an account</t>
+  </si>
+  <si>
+    <t>the system automatically assign user IDs in a simple, consistent format (e.g., U001, U002)</t>
+  </si>
+  <si>
+    <t>SRS-ID-002.2</t>
+  </si>
+  <si>
+    <t>LH-CRS-NOTIFICATIONS-001</t>
+  </si>
+  <si>
+    <t>users can follow specific categories to receive notifications when new content is added</t>
+  </si>
+  <si>
+    <t>LH-CRS-NOTIFICATIONS-002</t>
+  </si>
+  <si>
+    <t>The system must notify users within the website interface when new content is added to a followed category.</t>
+  </si>
+  <si>
+    <t>NOTIFICATIONS</t>
+  </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t>Mahmoud Abdelmageed</t>
+  </si>
+  <si>
+    <t>created Notifications and ID CONSTRAINTS RTM (CRS to SRS) and (SRS to Test Cases)</t>
+  </si>
+  <si>
+    <t>24/4/2026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -796,8 +913,78 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF404040"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,6 +1043,42 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor theme="0" tint="-0.34998626667073579"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.34998626667073579"/>
       </patternFill>
     </fill>
   </fills>
@@ -986,7 +1209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -1052,7 +1275,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -1087,7 +1309,6 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1133,67 +1354,128 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="13" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1345,6 +1627,290 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1592,262 +2158,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0"/>
-        </horizontal>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1862,39 +2172,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A1:F22" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41">
-  <autoFilter ref="A1:F22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table27" displayName="Table27" ref="A1:F22" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" headerRowBorderDxfId="30" tableBorderDxfId="31">
+  <autoFilter ref="A1:F22" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="CRS ID " dataDxfId="40"/>
-    <tableColumn id="2" name="CRS Description" dataDxfId="39"/>
-    <tableColumn id="3" name="SRS ID" dataDxfId="38"/>
-    <tableColumn id="4" name="SRS Description" dataDxfId="37"/>
-    <tableColumn id="5" name="Status (CRS-SRS)" dataDxfId="36"/>
-    <tableColumn id="6" name="Comments/Gaps" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CRS ID " dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CRS Description" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SRS ID" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SRS Description" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Status (CRS-SRS)" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Comments/Gaps" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A1:F48" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
-  <autoFilter ref="A1:F48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table26" displayName="Table26" ref="A1:F64" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40">
+  <autoFilter ref="A1:F64" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="SRS ID" dataDxfId="30"/>
-    <tableColumn id="2" name="SRS Description" dataDxfId="29"/>
-    <tableColumn id="3" name="Test Case ID" dataDxfId="28"/>
-    <tableColumn id="4" name="Test Title" dataDxfId="27"/>
-    <tableColumn id="5" name="Test Result" dataDxfId="26"/>
-    <tableColumn id="6" name="Status (Test)" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="SRS ID" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SRS Description" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Test Case ID" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Test Title" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Test Result" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Status (Test)" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1932,9 +2242,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1969,7 +2279,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2004,7 +2314,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2177,26 +2487,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PTG22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:PTG31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="25.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31" style="2" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="2"/>
+    <col min="2" max="2" width="40.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="2"/>
     <col min="4" max="4" width="46" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="25.7109375" style="2"/>
+    <col min="5" max="5" width="17.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="25.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11343" s="1" customFormat="1" ht="40.5">
+    <row r="1" spans="1:11343" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -2216,7 +2526,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11343" ht="25.5">
+    <row r="2" spans="1:11343" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2232,11 +2542,11 @@
       <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:11343" ht="38.25">
+    <row r="3" spans="1:11343" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2252,9 +2562,9 @@
       <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="46"/>
+      <c r="G3" s="44"/>
     </row>
-    <row r="4" spans="1:11343" ht="38.25">
+    <row r="4" spans="1:11343" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2270,9 +2580,9 @@
       <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="46"/>
+      <c r="G4" s="44"/>
     </row>
-    <row r="5" spans="1:11343" ht="25.5">
+    <row r="5" spans="1:11343" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -2289,9 +2599,9 @@
         <v>28</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="47"/>
+      <c r="G5" s="45"/>
     </row>
-    <row r="6" spans="1:11343" customFormat="1" ht="15">
+    <row r="6" spans="1:11343" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -2300,7 +2610,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
     </row>
-    <row r="7" spans="1:11343" customFormat="1" ht="38.25">
+    <row r="7" spans="1:11343" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>61</v>
       </c>
@@ -2317,15 +2627,11 @@
         <v>28</v>
       </c>
       <c r="F7" s="24"/>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
     </row>
-    <row r="8" spans="1:11343" customFormat="1" ht="38.25">
+    <row r="8" spans="1:11343" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>65</v>
       </c>
@@ -2342,13 +2648,9 @@
         <v>28</v>
       </c>
       <c r="F8" s="24"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="G8" s="46"/>
     </row>
-    <row r="9" spans="1:11343" customFormat="1" ht="38.25">
+    <row r="9" spans="1:11343" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>69</v>
       </c>
@@ -2364,25 +2666,21 @@
       <c r="E9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="46"/>
     </row>
-    <row r="10" spans="1:11343" s="22" customFormat="1" ht="15">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
+    <row r="10" spans="1:11343" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
@@ -13716,7 +14014,7 @@
       <c r="PTF10" s="20"/>
       <c r="PTG10" s="20"/>
     </row>
-    <row r="11" spans="1:11343" customFormat="1" ht="48.75" customHeight="1">
+    <row r="11" spans="1:11343" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>111</v>
       </c>
@@ -13732,16 +14030,12 @@
       <c r="E11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="42" t="s">
+      <c r="F11" s="25"/>
+      <c r="G11" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
     </row>
-    <row r="12" spans="1:11343" customFormat="1" ht="47.25" customHeight="1">
+    <row r="12" spans="1:11343" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>112</v>
       </c>
@@ -13757,23 +14051,20 @@
       <c r="E12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="41"/>
     </row>
-    <row r="13" spans="1:11343">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
+    <row r="13" spans="1:11343" x14ac:dyDescent="0.3">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="31"/>
     </row>
-    <row r="14" spans="1:11343" ht="45" customHeight="1">
+    <row r="14" spans="1:11343" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>114</v>
       </c>
@@ -13789,12 +14080,12 @@
       <c r="E14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="42" t="s">
+      <c r="F14" s="25"/>
+      <c r="G14" s="40" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:11343" ht="38.25">
+    <row r="15" spans="1:11343" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>114</v>
       </c>
@@ -13810,10 +14101,10 @@
       <c r="E15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="43"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="41"/>
     </row>
-    <row r="16" spans="1:11343" ht="51">
+    <row r="16" spans="1:11343" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>114</v>
       </c>
@@ -13829,10 +14120,10 @@
       <c r="E16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="41"/>
     </row>
-    <row r="17" spans="1:7" ht="38.25">
+    <row r="17" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>114</v>
       </c>
@@ -13848,10 +14139,10 @@
       <c r="E17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="43"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="41"/>
     </row>
-    <row r="18" spans="1:7" ht="38.25">
+    <row r="18" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>115</v>
       </c>
@@ -13867,10 +14158,10 @@
       <c r="E18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="43"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="41"/>
     </row>
-    <row r="19" spans="1:7" ht="38.25">
+    <row r="19" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>116</v>
       </c>
@@ -13886,10 +14177,10 @@
       <c r="E19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="43"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="41"/>
     </row>
-    <row r="20" spans="1:7" ht="38.25">
+    <row r="20" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>117</v>
       </c>
@@ -13905,10 +14196,10 @@
       <c r="E20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="41"/>
     </row>
-    <row r="21" spans="1:7" ht="51">
+    <row r="21" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>118</v>
       </c>
@@ -13924,10 +14215,10 @@
       <c r="E21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="43"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="41"/>
     </row>
-    <row r="22" spans="1:7" ht="51">
+    <row r="22" spans="1:7" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
         <v>119</v>
       </c>
@@ -13943,123 +14234,312 @@
       <c r="E22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="44"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="42"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+    </row>
+    <row r="24" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="68" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="C24" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="E24" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="68"/>
+      <c r="G24" s="80" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="69" t="s">
+        <v>210</v>
+      </c>
+      <c r="B25" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>197</v>
+      </c>
+      <c r="E25" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="67"/>
+      <c r="G25" s="81"/>
+    </row>
+    <row r="26" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" s="68" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="E26" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="68"/>
+      <c r="G26" s="81"/>
+    </row>
+    <row r="27" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="75" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="70" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="71" t="s">
+        <v>199</v>
+      </c>
+      <c r="E27" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="67"/>
+      <c r="G27" s="82"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+    </row>
+    <row r="29" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" s="60" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="D29" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="68"/>
+      <c r="G29" s="89" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="B30" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" s="79" t="s">
+        <v>207</v>
+      </c>
+      <c r="D30" s="79" t="s">
+        <v>201</v>
+      </c>
+      <c r="E30" s="67" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="67"/>
+      <c r="G30" s="90"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="G29:G30"/>
     <mergeCell ref="G14:G22"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="G11:G12"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:F4 B7:E8 A23:F1048576">
-    <cfRule type="expression" priority="25">
-      <formula>ISBLANK($C2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:XFD2 A3:F5 H3:XFD5 A23:F1048576 H13:XFD18">
-    <cfRule type="expression" dxfId="24" priority="24">
+  <conditionalFormatting sqref="A1:F4 B7:E8 A24:B24 F24 A27:F27 A29:F30 A32:F1048576">
+    <cfRule type="expression" priority="31">
       <formula>ISBLANK($C2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:F5">
-    <cfRule type="expression" priority="28">
+    <cfRule type="expression" priority="34">
       <formula>ISBLANK($C12)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7 G11">
-    <cfRule type="expression" dxfId="23" priority="15">
+  <conditionalFormatting sqref="A2:XFD2 A3:F5 H3:XFD5 H13:XFD18 A24:B25 A29:F30 E24:F25 E27:F27 B26:B27 A32:F1048576">
+    <cfRule type="expression" dxfId="23" priority="30">
+      <formula>ISBLANK($C2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:B9">
+    <cfRule type="expression" dxfId="22" priority="24">
       <formula>ISBLANK($C7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E9">
-    <cfRule type="expression" dxfId="22" priority="22">
+  <conditionalFormatting sqref="B11:B12">
+    <cfRule type="expression" dxfId="21" priority="17">
+      <formula>ISBLANK($C11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:B22">
+    <cfRule type="expression" dxfId="20" priority="8">
+      <formula>ISBLANK($C14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:E9 E24">
+    <cfRule type="expression" priority="37">
+      <formula>ISBLANK($C12)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:E12 A25:B25 F25">
+    <cfRule type="expression" priority="20">
+      <formula>ISBLANK($C13)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:E22">
+    <cfRule type="expression" priority="11">
+      <formula>ISBLANK($C16)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:C9">
+    <cfRule type="expression" dxfId="19" priority="26">
       <formula>ISBLANK($C7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C9">
-    <cfRule type="expression" dxfId="21" priority="20">
+  <conditionalFormatting sqref="C11:C12">
+    <cfRule type="expression" dxfId="18" priority="18">
+      <formula>ISBLANK($C11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:C22">
+    <cfRule type="expression" dxfId="17" priority="9">
+      <formula>ISBLANK($C14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:D9">
+    <cfRule type="expression" dxfId="16" priority="22">
       <formula>ISBLANK($C7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B9">
-    <cfRule type="expression" dxfId="20" priority="18">
+  <conditionalFormatting sqref="D11:D12">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>ISBLANK($C11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D22">
+    <cfRule type="expression" dxfId="14" priority="7">
+      <formula>ISBLANK($C14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:E9">
+    <cfRule type="expression" dxfId="13" priority="28">
       <formula>ISBLANK($C7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D9">
-    <cfRule type="expression" dxfId="19" priority="16">
+  <conditionalFormatting sqref="E11:E12">
+    <cfRule type="expression" dxfId="12" priority="19">
+      <formula>ISBLANK($C11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E22">
+    <cfRule type="expression" dxfId="11" priority="10">
+      <formula>ISBLANK($C14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7 G11">
+    <cfRule type="expression" dxfId="10" priority="21">
       <formula>ISBLANK($C7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:E9">
-    <cfRule type="expression" priority="31">
-      <formula>ISBLANK($C12)</formula>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>ISBLANK($C14)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E12">
-    <cfRule type="expression" dxfId="18" priority="13">
-      <formula>ISBLANK($C11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C12">
-    <cfRule type="expression" dxfId="17" priority="12">
-      <formula>ISBLANK($C11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B12">
-    <cfRule type="expression" dxfId="16" priority="11">
-      <formula>ISBLANK($C11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D12">
-    <cfRule type="expression" dxfId="15" priority="10">
-      <formula>ISBLANK($C11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:E12">
-    <cfRule type="expression" priority="14">
-      <formula>ISBLANK($C13)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G23:XFD1048576 H19:XFD22">
-    <cfRule type="expression" dxfId="14" priority="38">
+  <conditionalFormatting sqref="H19:XFD21 G32:XFD1048576 H23:XFD31">
+    <cfRule type="expression" dxfId="8" priority="44">
       <formula>ISBLANK($C23)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14">
-    <cfRule type="expression" dxfId="13" priority="9">
-      <formula>ISBLANK($C14)</formula>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:B22">
-    <cfRule type="expression" dxfId="12" priority="2">
-      <formula>ISBLANK($C14)</formula>
+  <conditionalFormatting sqref="F26 B26:B27 E25:E26">
+    <cfRule type="expression" priority="49">
+      <formula>ISBLANK(#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D22">
-    <cfRule type="expression" dxfId="11" priority="1">
-      <formula>ISBLANK($C14)</formula>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="expression" dxfId="7" priority="53">
+      <formula>ISBLANK($C27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E22">
-    <cfRule type="expression" dxfId="10" priority="4">
-      <formula>ISBLANK($C14)</formula>
+  <conditionalFormatting sqref="H22:XFD22">
+    <cfRule type="expression" dxfId="6" priority="56">
+      <formula>ISBLANK($C27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C22">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>ISBLANK($C14)</formula>
+  <conditionalFormatting sqref="A26:B26">
+    <cfRule type="expression" priority="3">
+      <formula>ISBLANK($C27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:E22">
-    <cfRule type="expression" priority="5">
-      <formula>ISBLANK($C16)</formula>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>ISBLANK($C26)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>ISBLANK($C24)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E9 E11:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E9 E11:E1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Draft, Approved, Under Review, Rejected"</formula1>
     </dataValidation>
   </dataValidations>
@@ -14072,25 +14552,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A48"/>
+    <sheetView topLeftCell="A39" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30:G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="25.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="2"/>
-    <col min="2" max="2" width="50.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="25.7109375" style="2"/>
-    <col min="7" max="7" width="23.140625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="25.7109375" style="2"/>
+    <col min="1" max="1" width="25.6640625" style="2"/>
+    <col min="2" max="2" width="50.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="25.6640625" style="2"/>
+    <col min="7" max="7" width="23.109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="25.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14110,7 +14590,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5">
+    <row r="2" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -14123,11 +14603,11 @@
       <c r="D2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="47" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25.5">
+    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -14140,9 +14620,9 @@
       <c r="D3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="50"/>
+      <c r="G3" s="48"/>
     </row>
-    <row r="4" spans="1:7" ht="25.5">
+    <row r="4" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -14155,9 +14635,9 @@
       <c r="D4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="50"/>
+      <c r="G4" s="48"/>
     </row>
-    <row r="5" spans="1:7" ht="25.5">
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -14170,9 +14650,9 @@
       <c r="D5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="50"/>
+      <c r="G5" s="48"/>
     </row>
-    <row r="6" spans="1:7" ht="25.5">
+    <row r="6" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -14185,9 +14665,9 @@
       <c r="D6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="50"/>
+      <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:7" ht="25.5">
+    <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -14200,9 +14680,9 @@
       <c r="D7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="50"/>
+      <c r="G7" s="48"/>
     </row>
-    <row r="8" spans="1:7" ht="25.5">
+    <row r="8" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -14215,9 +14695,9 @@
       <c r="D8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="50"/>
+      <c r="G8" s="48"/>
     </row>
-    <row r="9" spans="1:7" ht="25.5">
+    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -14230,9 +14710,9 @@
       <c r="D9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="50"/>
+      <c r="G9" s="48"/>
     </row>
-    <row r="10" spans="1:7" ht="25.5">
+    <row r="10" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -14245,9 +14725,9 @@
       <c r="D10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="50"/>
+      <c r="G10" s="48"/>
     </row>
-    <row r="11" spans="1:7" ht="25.5">
+    <row r="11" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -14260,9 +14740,9 @@
       <c r="D11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="50"/>
+      <c r="G11" s="48"/>
     </row>
-    <row r="12" spans="1:7" ht="25.5">
+    <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -14275,9 +14755,9 @@
       <c r="D12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="50"/>
+      <c r="G12" s="48"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -14290,9 +14770,9 @@
       <c r="D13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="50"/>
+      <c r="G13" s="48"/>
     </row>
-    <row r="14" spans="1:7" ht="25.5">
+    <row r="14" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -14305,9 +14785,9 @@
       <c r="D14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="50"/>
+      <c r="G14" s="48"/>
     </row>
-    <row r="15" spans="1:7" ht="25.5">
+    <row r="15" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -14322,223 +14802,223 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="51"/>
+      <c r="G15" s="49"/>
     </row>
-    <row r="16" spans="1:7" customFormat="1" ht="15">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
+    <row r="16" spans="1:7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
       <c r="G16" s="22"/>
     </row>
-    <row r="17" spans="1:7" customFormat="1" ht="38.25">
+    <row r="17" spans="1:7" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>75</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="52" t="s">
+      <c r="G17" s="50" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:7" customFormat="1" ht="38.25">
+    <row r="18" spans="1:7" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="27" t="s">
         <v>77</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="53"/>
+      <c r="G18" s="51"/>
     </row>
-    <row r="19" spans="1:7" customFormat="1" ht="38.25">
+    <row r="19" spans="1:7" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="27" t="s">
         <v>79</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="53"/>
+      <c r="G19" s="51"/>
     </row>
-    <row r="20" spans="1:7" customFormat="1" ht="63.75">
+    <row r="20" spans="1:7" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="29" t="s">
         <v>81</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="53"/>
+      <c r="G20" s="51"/>
     </row>
-    <row r="21" spans="1:7" customFormat="1" ht="15">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
+    <row r="21" spans="1:7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="1:7" customFormat="1" ht="108.75" customHeight="1">
+    <row r="22" spans="1:7" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="38" t="s">
         <v>100</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="52" t="s">
+      <c r="G22" s="50" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="78" customHeight="1">
+    <row r="23" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="38" t="s">
         <v>101</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="G23" s="55"/>
+      <c r="G23" s="52"/>
     </row>
-    <row r="24" spans="1:7" ht="78" customHeight="1">
+    <row r="24" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="38" t="s">
         <v>102</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="G24" s="55"/>
+      <c r="G24" s="52"/>
     </row>
-    <row r="25" spans="1:7" ht="67.5" customHeight="1">
+    <row r="25" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D25" s="39" t="s">
         <v>103</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="G25" s="55"/>
+      <c r="G25" s="52"/>
     </row>
-    <row r="26" spans="1:7" ht="59.25" customHeight="1">
+    <row r="26" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="38" t="s">
         <v>104</v>
       </c>
       <c r="E26" s="3"/>
-      <c r="G26" s="55"/>
+      <c r="G26" s="52"/>
     </row>
-    <row r="27" spans="1:7" ht="84">
+    <row r="27" spans="1:7" ht="63" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="38" t="s">
         <v>106</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="G27" s="55"/>
+      <c r="G27" s="52"/>
     </row>
-    <row r="28" spans="1:7" ht="84">
+    <row r="28" spans="1:7" ht="63" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="38" t="s">
         <v>107</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="G28" s="56"/>
+      <c r="G28" s="53"/>
     </row>
-    <row r="29" spans="1:7" ht="15">
-      <c r="A29" s="31"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
+    <row r="29" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:7" ht="38.25" customHeight="1">
+    <row r="30" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>129</v>
@@ -14547,13 +15027,13 @@
         <v>145</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="G30" s="50" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="38.25">
+    <row r="31" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>121</v>
       </c>
@@ -14564,11 +15044,11 @@
         <v>146</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G31" s="55"/>
     </row>
-    <row r="32" spans="1:7" ht="38.25">
+    <row r="32" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>122</v>
       </c>
@@ -14579,11 +15059,11 @@
         <v>147</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G32" s="55"/>
     </row>
-    <row r="33" spans="1:7" ht="38.25">
+    <row r="33" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>123</v>
       </c>
@@ -14594,11 +15074,11 @@
         <v>148</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G33" s="55"/>
     </row>
-    <row r="34" spans="1:7" ht="38.25">
+    <row r="34" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>124</v>
       </c>
@@ -14609,11 +15089,11 @@
         <v>149</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G34" s="55"/>
     </row>
-    <row r="35" spans="1:7" ht="38.25">
+    <row r="35" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>124</v>
       </c>
@@ -14624,11 +15104,11 @@
         <v>150</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G35" s="55"/>
     </row>
-    <row r="36" spans="1:7" ht="38.25">
+    <row r="36" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>124</v>
       </c>
@@ -14639,11 +15119,11 @@
         <v>151</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G36" s="55"/>
     </row>
-    <row r="37" spans="1:7" ht="17.25" customHeight="1">
+    <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>125</v>
       </c>
@@ -14654,11 +15134,11 @@
         <v>152</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G37" s="55"/>
     </row>
-    <row r="38" spans="1:7" ht="38.25">
+    <row r="38" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>125</v>
       </c>
@@ -14669,11 +15149,11 @@
         <v>153</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G38" s="55"/>
     </row>
-    <row r="39" spans="1:7" ht="38.25">
+    <row r="39" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>125</v>
       </c>
@@ -14684,11 +15164,11 @@
         <v>154</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G39" s="55"/>
     </row>
-    <row r="40" spans="1:7" ht="38.25">
+    <row r="40" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>126</v>
       </c>
@@ -14699,11 +15179,11 @@
         <v>155</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G40" s="55"/>
     </row>
-    <row r="41" spans="1:7" ht="38.25">
+    <row r="41" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>126</v>
       </c>
@@ -14714,11 +15194,11 @@
         <v>156</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G41" s="55"/>
     </row>
-    <row r="42" spans="1:7" ht="38.25">
+    <row r="42" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>126</v>
       </c>
@@ -14729,11 +15209,11 @@
         <v>157</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G42" s="55"/>
     </row>
-    <row r="43" spans="1:7" ht="38.25">
+    <row r="43" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>126</v>
       </c>
@@ -14744,11 +15224,11 @@
         <v>158</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G43" s="55"/>
     </row>
-    <row r="44" spans="1:7" ht="38.25">
+    <row r="44" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>126</v>
       </c>
@@ -14759,11 +15239,11 @@
         <v>159</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G44" s="55"/>
     </row>
-    <row r="45" spans="1:7" ht="38.25">
+    <row r="45" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>127</v>
       </c>
@@ -14774,11 +15254,11 @@
         <v>160</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G45" s="55"/>
     </row>
-    <row r="46" spans="1:7" ht="38.25">
+    <row r="46" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>127</v>
       </c>
@@ -14789,77 +15269,189 @@
         <v>161</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G46" s="55"/>
     </row>
-    <row r="47" spans="1:7" ht="38.25">
+    <row r="47" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>162</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="G47" s="55"/>
+        <v>180</v>
+      </c>
+      <c r="G47" s="56"/>
     </row>
-    <row r="48" spans="1:7" ht="38.25">
-      <c r="A48" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="G48" s="56"/>
+    <row r="48" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="31"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+    </row>
+    <row r="49" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="G49" s="86" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B50" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="G50" s="87"/>
+    </row>
+    <row r="51" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B51" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="G51" s="88"/>
+    </row>
+    <row r="52" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="31"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="83"/>
+    </row>
+    <row r="53" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="G53" s="84" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G54" s="85"/>
+    </row>
+    <row r="55" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="31"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+    </row>
+    <row r="56" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="D62" s="6"/>
+    </row>
+    <row r="63" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="D63" s="6"/>
+    </row>
+    <row r="64" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="D64" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="G30:G47"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="G53:G54"/>
     <mergeCell ref="G2:G15"/>
     <mergeCell ref="G17:G20"/>
     <mergeCell ref="G22:G28"/>
-    <mergeCell ref="G30:G48"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E1:E28 E49:E1048576">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="E1:E64">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",E29)))</formula>
+  <conditionalFormatting sqref="E65:E1048576">
+    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",E65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",E29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:E48">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",E30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",E30)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",E65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass, Fail, Blocked, N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Not Started, In Progress, Closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -14871,19 +15463,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="21.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="21.85546875" style="8"/>
+    <col min="1" max="16384" width="21.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>44</v>
       </c>
@@ -14891,34 +15483,34 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="8">
         <f>COUNTA(CRS_to_SRS!A2:A110)</f>
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="8">
-        <f>COUNTA(SRS_to_Test!A2:A133)</f>
-        <v>44</v>
+        <f>COUNTA(SRS_to_Test!A2:A149)</f>
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="8">
-        <f>COUNTIF(SRS_to_Test!E2:E133, "Pass")</f>
+        <f>COUNTIF(SRS_to_Test!E2:E149, "Pass")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>49</v>
       </c>
@@ -14927,8 +15519,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="9" customFormat="1"/>
-    <row r="7" spans="1:2" ht="21">
+    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>50</v>
       </c>
@@ -14936,22 +15528,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="8">
         <f>COUNTIF(CRS_to_SRS!C2:C110, "")</f>
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B9" s="8">
-        <f>COUNTIF(SRS_to_Test!C2:C133, "")</f>
-        <v>88</v>
+        <f>COUNTIF(SRS_to_Test!C2:C149, "")</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -14960,25 +15552,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="11" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="11" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
@@ -14992,7 +15584,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75">
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>57</v>
       </c>
@@ -15006,7 +15598,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="37.5">
+    <row r="3" spans="1:6" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>82</v>
       </c>
@@ -15020,7 +15612,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="56.25">
+    <row r="4" spans="1:6" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>108</v>
       </c>
@@ -15034,24 +15626,38 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="56.25">
+    <row r="5" spans="1:6" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>187</v>
-      </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="6" spans="1:6" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="78" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="77" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F10" s="20"/>
     </row>
-    <row r="17" spans="2:4" ht="21">
+    <row r="17" spans="2:4" ht="21" x14ac:dyDescent="0.4">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -15063,19 +15669,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.45" customHeight="1">
+    <row r="1" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>42</v>
       </c>
@@ -15083,37 +15689,37 @@
       <c r="C1" s="54"/>
       <c r="D1" s="54"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="54"/>
       <c r="B2" s="54"/>
       <c r="C2" s="54"/>
       <c r="D2" s="54"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="54"/>
       <c r="B3" s="54"/>
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="54"/>
       <c r="B4" s="54"/>
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="54"/>
       <c r="B5" s="54"/>
       <c r="C5" s="54"/>
       <c r="D5" s="54"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="54"/>
       <c r="B6" s="54"/>
       <c r="C6" s="54"/>
       <c r="D6" s="54"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="54"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>

</xml_diff>